<commit_message>
Java_detailed.xlsx file polished a bit
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/Java_detailed.xlsx
+++ b/src/main/java/org/eminera/_syllabus/Java_detailed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eminera\java_group_1\classes\src\main\java\org\eminera\_syllabus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840CD804-DA46-4F81-9F7F-522CB566D7B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98479EB-7E17-4A6C-AF43-98EA69BA1553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>A. Basic / Syntax</t>
   </si>
@@ -45,9 +45,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>YouTube</t>
-  </si>
-  <si>
     <t>Intro to ICT</t>
   </si>
   <si>
@@ -63,14 +60,26 @@
     <t>Control Flow -  Loops (while, do-while, enhanced for loop)</t>
   </si>
   <si>
-    <t>done</t>
+    <t>YouTube link</t>
+  </si>
+  <si>
+    <t>https://youtu.be/3Q7s1cpByuk</t>
+  </si>
+  <si>
+    <t>https://youtu.be/9fIwJtlF_Dg</t>
+  </si>
+  <si>
+    <t>https://youtu.be/tqJZedXiqeI</t>
+  </si>
+  <si>
+    <t>https://youtu.be/yNGEqPdB944</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,17 +94,36 @@
       <family val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -136,42 +164,59 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,126 +498,142 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="63" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="7">
+        <v>2</v>
+      </c>
+      <c r="E2" s="13">
+        <v>44088</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="10">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="10">
-        <v>2</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="10">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="7">
         <f>B2+1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="10">
+      <c r="C3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7">
         <v>2</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="11"/>
+      <c r="E3" s="15">
+        <v>44093</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="10">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="7">
         <f t="shared" ref="B4:B5" si="0">B3+1</f>
         <v>3</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="10">
+      <c r="C4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="7">
         <v>2</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="11"/>
+      <c r="E4" s="16">
+        <v>44095</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="10">
+    <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="C5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="7">
         <v>2</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="11"/>
+      <c r="E5" s="16">
+        <v>44100</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="10">
+    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="7">
         <f>B5+1</f>
         <v>5</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="C6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="7">
         <v>2</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="E6" s="16">
+        <v>44084</v>
+      </c>
+      <c r="F6" s="9"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{330D97D7-94E1-441E-A870-70DAC2F1FEF2}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{F357F35B-9293-49C1-AD7E-6FB9B1621200}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{FA67CD3A-6F07-4D84-B1F2-3770C7164B19}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{8A1DF1EF-BBBC-436D-B838-6CFA59F90FE0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"10-Oct-2020 lesson's details added"
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/Java_detailed.xlsx
+++ b/src/main/java/org/eminera/_syllabus/Java_detailed.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eminera\java_group_1\classes\src\main\java\org\eminera\_syllabus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\elvin_taghizade\IdeaProjects\mine\git\java-course-1-classes\src\main\java\org\eminera\_syllabus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98479EB-7E17-4A6C-AF43-98EA69BA1553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>A. Basic / Syntax</t>
   </si>
@@ -73,13 +72,16 @@
   </si>
   <si>
     <t>https://youtu.be/yNGEqPdB944</t>
+  </si>
+  <si>
+    <t>https://youtu.be/OgDodkukz9U</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,9 +195,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -214,6 +213,7 @@
     <xf numFmtId="15" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -494,14 +494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -512,7 +512,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="28.5">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -532,7 +532,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -545,95 +545,98 @@
       <c r="D2" s="7">
         <v>2</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>44088</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
+    <row r="3" spans="1:6" ht="15">
+      <c r="A3" s="9"/>
       <c r="B3" s="7">
         <f>B2+1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="7">
         <v>2</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>44093</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
+    <row r="4" spans="1:6" ht="15">
+      <c r="A4" s="9"/>
       <c r="B4" s="7">
         <f t="shared" ref="B4:B5" si="0">B3+1</f>
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="7">
         <v>2</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <v>44095</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
+    <row r="5" spans="1:6" ht="38.25">
+      <c r="A5" s="9"/>
       <c r="B5" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="7">
         <v>2</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="15">
         <v>44100</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
+    <row r="6" spans="1:6" ht="26.25">
+      <c r="A6" s="9"/>
       <c r="B6" s="7">
         <f>B5+1</f>
         <v>5</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="7">
         <v>2</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>44084</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="16" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{330D97D7-94E1-441E-A870-70DAC2F1FEF2}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{F357F35B-9293-49C1-AD7E-6FB9B1621200}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{FA67CD3A-6F07-4D84-B1F2-3770C7164B19}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{8A1DF1EF-BBBC-436D-B838-6CFA59F90FE0}"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"lesson #6 video record uploaded into youtube and link attached in details.xlsx file under syllabus folder"
</commit_message>
<xml_diff>
--- a/src/main/java/org/eminera/_syllabus/Java_detailed.xlsx
+++ b/src/main/java/org/eminera/_syllabus/Java_detailed.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>A. Basic / Syntax</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>https://youtu.be/OgDodkukz9U</t>
+  </si>
+  <si>
+    <t>https://youtu.be/G0B2xyAF3RY</t>
+  </si>
+  <si>
+    <t>Methods in Java</t>
   </si>
 </sst>
 </file>
@@ -495,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -508,7 +514,7 @@
     <col min="3" max="3" width="30.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -626,6 +632,25 @@
       </c>
       <c r="F6" s="16" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15">
+      <c r="A7" s="9"/>
+      <c r="B7" s="7">
+        <f>B6+1</f>
+        <v>6</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="15">
+        <v>44088</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -635,8 +660,9 @@
     <hyperlink ref="F2" r:id="rId3"/>
     <hyperlink ref="F5" r:id="rId4"/>
     <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>